<commit_message>
Added Cantonese and Algerian to lang codes table and fixed some that had more than one name, also created file to map group and color
</commit_message>
<xml_diff>
--- a/utils/lang_codes.xlsx
+++ b/utils/lang_codes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aturt\Documents\typology_of_crosslingual\data_exploration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aturt\Documents\typology_of_crosslingual\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="2104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2280" uniqueCount="2109">
   <si>
     <t>ISO 639-2 Code</t>
   </si>
@@ -5267,12 +5267,6 @@
     <t>es</t>
   </si>
   <si>
-    <t>Spanish; Castilian</t>
-  </si>
-  <si>
-    <t>espagnol; castillan</t>
-  </si>
-  <si>
     <t>Spanisch</t>
   </si>
   <si>
@@ -6336,13 +6330,34 @@
   </si>
   <si>
     <t>Zazaki</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>espagnol</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>zh-yue</t>
+  </si>
+  <si>
+    <t>Cantonese</t>
+  </si>
+  <si>
+    <t>ar-dz</t>
+  </si>
+  <si>
+    <t>Algerian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6360,6 +6375,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292E"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -6384,7 +6405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -6433,11 +6454,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6451,6 +6487,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -6737,10 +6781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E548"/>
+  <dimension ref="A1:E550"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
+      <selection activeCell="G552" sqref="G552"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6954,16 +6998,16 @@
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -6971,10 +7015,10 @@
       <c r="A15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -7136,16 +7180,16 @@
       <c r="A26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -7153,10 +7197,10 @@
       <c r="A27" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -7461,16 +7505,16 @@
       <c r="A47" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="9" t="s">
         <v>197</v>
       </c>
     </row>
@@ -7478,10 +7522,10 @@
       <c r="A48" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
@@ -7705,16 +7749,16 @@
       <c r="A63" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E63" s="9" t="s">
         <v>261</v>
       </c>
     </row>
@@ -7722,10 +7766,10 @@
       <c r="A64" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
@@ -7842,16 +7886,16 @@
       <c r="A72" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E72" s="9" t="s">
         <v>298</v>
       </c>
     </row>
@@ -7859,10 +7903,10 @@
       <c r="A73" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
     </row>
     <row r="74" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
@@ -7990,16 +8034,16 @@
       <c r="A82" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C82" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E82" s="9" t="s">
         <v>336</v>
       </c>
     </row>
@@ -8007,10 +8051,10 @@
       <c r="A83" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B83" s="6"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
     </row>
     <row r="84" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
@@ -8080,16 +8124,16 @@
       <c r="A88" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="9" t="s">
         <v>360</v>
       </c>
     </row>
@@ -8097,10 +8141,10 @@
       <c r="A89" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="6"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
@@ -8446,16 +8490,16 @@
       <c r="A112" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="C112" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="D112" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="E112" s="5" t="s">
+      <c r="E112" s="9" t="s">
         <v>459</v>
       </c>
     </row>
@@ -8463,25 +8507,25 @@
       <c r="A113" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="B113" s="6"/>
-      <c r="C113" s="6"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="6"/>
+      <c r="B113" s="10"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B114" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="C114" s="5" t="s">
+      <c r="C114" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D114" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="E114" s="5" t="s">
+      <c r="E114" s="9" t="s">
         <v>336</v>
       </c>
     </row>
@@ -8489,10 +8533,10 @@
       <c r="A115" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="B115" s="6"/>
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="6"/>
+      <c r="B115" s="10"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
@@ -8590,16 +8634,16 @@
       <c r="A122" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B122" s="9" t="s">
         <v>487</v>
       </c>
-      <c r="C122" s="5" t="s">
+      <c r="C122" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="D122" s="5" t="s">
+      <c r="D122" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="E122" s="5" t="s">
+      <c r="E122" s="9" t="s">
         <v>490</v>
       </c>
     </row>
@@ -8607,10 +8651,10 @@
       <c r="A123" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="B123" s="6"/>
-      <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
-      <c r="E123" s="6"/>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
     </row>
     <row r="124" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
@@ -8738,16 +8782,16 @@
       <c r="A132" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="B132" s="5" t="s">
+      <c r="B132" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="C132" s="5" t="s">
+      <c r="C132" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D132" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="E132" s="5" t="s">
+      <c r="E132" s="9" t="s">
         <v>528</v>
       </c>
     </row>
@@ -8755,10 +8799,10 @@
       <c r="A133" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="B133" s="6"/>
-      <c r="C133" s="6"/>
-      <c r="D133" s="6"/>
-      <c r="E133" s="6"/>
+      <c r="B133" s="10"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
     </row>
     <row r="134" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
@@ -8841,16 +8885,16 @@
       <c r="A139" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="B139" s="5" t="s">
+      <c r="B139" s="9" t="s">
         <v>549</v>
       </c>
-      <c r="C139" s="5" t="s">
-        <v>550</v>
-      </c>
-      <c r="D139" s="5" t="s">
+      <c r="C139" s="9" t="s">
+        <v>2104</v>
+      </c>
+      <c r="D139" s="9" t="s">
         <v>551</v>
       </c>
-      <c r="E139" s="5" t="s">
+      <c r="E139" s="9" t="s">
         <v>552</v>
       </c>
     </row>
@@ -8858,10 +8902,10 @@
       <c r="A140" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="B140" s="6"/>
-      <c r="C140" s="6"/>
-      <c r="D140" s="6"/>
-      <c r="E140" s="6"/>
+      <c r="B140" s="10"/>
+      <c r="C140" s="10"/>
+      <c r="D140" s="10"/>
+      <c r="E140" s="10"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
@@ -8948,16 +8992,16 @@
       <c r="A146" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B146" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C146" s="5" t="s">
+      <c r="C146" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D146" s="5" t="s">
+      <c r="D146" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E146" s="5" t="s">
+      <c r="E146" s="9" t="s">
         <v>197</v>
       </c>
     </row>
@@ -8965,10 +9009,10 @@
       <c r="A147" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B147" s="6"/>
-      <c r="C147" s="6"/>
-      <c r="D147" s="6"/>
-      <c r="E147" s="6"/>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
     </row>
     <row r="148" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
@@ -9038,16 +9082,16 @@
       <c r="A152" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="B152" s="5" t="s">
+      <c r="B152" s="9" t="s">
         <v>594</v>
       </c>
-      <c r="C152" s="5" t="s">
+      <c r="C152" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="D152" s="5" t="s">
+      <c r="D152" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="E152" s="5" t="s">
+      <c r="E152" s="9" t="s">
         <v>597</v>
       </c>
     </row>
@@ -9055,10 +9099,10 @@
       <c r="A153" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="B153" s="6"/>
-      <c r="C153" s="6"/>
-      <c r="D153" s="6"/>
-      <c r="E153" s="6"/>
+      <c r="B153" s="10"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
+      <c r="E153" s="10"/>
     </row>
     <row r="154" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
@@ -9158,16 +9202,16 @@
       <c r="A160" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="B160" s="5" t="s">
+      <c r="B160" s="9" t="s">
         <v>625</v>
       </c>
-      <c r="C160" s="5" t="s">
+      <c r="C160" s="9" t="s">
         <v>626</v>
       </c>
-      <c r="D160" s="5" t="s">
+      <c r="D160" s="9" t="s">
         <v>627</v>
       </c>
-      <c r="E160" s="5" t="s">
+      <c r="E160" s="9" t="s">
         <v>628</v>
       </c>
     </row>
@@ -9175,25 +9219,25 @@
       <c r="A161" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="B161" s="6"/>
-      <c r="C161" s="6"/>
-      <c r="D161" s="6"/>
-      <c r="E161" s="6"/>
+      <c r="B161" s="10"/>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="10"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="B162" s="5" t="s">
+      <c r="B162" s="9" t="s">
         <v>625</v>
       </c>
-      <c r="C162" s="5" t="s">
+      <c r="C162" s="9" t="s">
         <v>626</v>
       </c>
-      <c r="D162" s="5" t="s">
+      <c r="D162" s="9" t="s">
         <v>627</v>
       </c>
-      <c r="E162" s="5" t="s">
+      <c r="E162" s="9" t="s">
         <v>628</v>
       </c>
     </row>
@@ -9201,10 +9245,10 @@
       <c r="A163" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="B163" s="6"/>
-      <c r="C163" s="6"/>
-      <c r="D163" s="6"/>
-      <c r="E163" s="6"/>
+      <c r="B163" s="10"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
     </row>
     <row r="164" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
@@ -9379,16 +9423,16 @@
       <c r="A175" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="B175" s="5" t="s">
+      <c r="B175" s="9" t="s">
         <v>677</v>
       </c>
-      <c r="C175" s="5" t="s">
+      <c r="C175" s="9" t="s">
         <v>678</v>
       </c>
-      <c r="D175" s="5" t="s">
+      <c r="D175" s="9" t="s">
         <v>679</v>
       </c>
-      <c r="E175" s="5" t="s">
+      <c r="E175" s="9" t="s">
         <v>680</v>
       </c>
     </row>
@@ -9396,25 +9440,25 @@
       <c r="A176" s="4" t="s">
         <v>676</v>
       </c>
-      <c r="B176" s="6"/>
-      <c r="C176" s="6"/>
-      <c r="D176" s="6"/>
-      <c r="E176" s="6"/>
+      <c r="B176" s="10"/>
+      <c r="C176" s="10"/>
+      <c r="D176" s="10"/>
+      <c r="E176" s="10"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="B177" s="5" t="s">
+      <c r="B177" s="9" t="s">
         <v>487</v>
       </c>
-      <c r="C177" s="5" t="s">
+      <c r="C177" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="D177" s="5" t="s">
+      <c r="D177" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="E177" s="5" t="s">
+      <c r="E177" s="9" t="s">
         <v>490</v>
       </c>
     </row>
@@ -9422,10 +9466,10 @@
       <c r="A178" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="B178" s="6"/>
-      <c r="C178" s="6"/>
-      <c r="D178" s="6"/>
-      <c r="E178" s="6"/>
+      <c r="B178" s="10"/>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10"/>
+      <c r="E178" s="10"/>
     </row>
     <row r="179" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
@@ -9634,16 +9678,16 @@
       <c r="A192" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="B192" s="5" t="s">
+      <c r="B192" s="9" t="s">
         <v>549</v>
       </c>
-      <c r="C192" s="5" t="s">
+      <c r="C192" s="9" t="s">
         <v>550</v>
       </c>
-      <c r="D192" s="5" t="s">
+      <c r="D192" s="9" t="s">
         <v>551</v>
       </c>
-      <c r="E192" s="5" t="s">
+      <c r="E192" s="9" t="s">
         <v>552</v>
       </c>
     </row>
@@ -9651,10 +9695,10 @@
       <c r="A193" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="B193" s="6"/>
-      <c r="C193" s="6"/>
-      <c r="D193" s="6"/>
-      <c r="E193" s="6"/>
+      <c r="B193" s="10"/>
+      <c r="C193" s="10"/>
+      <c r="D193" s="10"/>
+      <c r="E193" s="10"/>
     </row>
     <row r="194" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
@@ -9980,16 +10024,16 @@
       <c r="A214" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B214" s="5" t="s">
+      <c r="B214" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C214" s="5" t="s">
+      <c r="C214" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D214" s="5" t="s">
+      <c r="D214" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E214" s="5" t="s">
+      <c r="E214" s="9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -9997,10 +10041,10 @@
       <c r="A215" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B215" s="6"/>
-      <c r="C215" s="6"/>
-      <c r="D215" s="6"/>
-      <c r="E215" s="6"/>
+      <c r="B215" s="10"/>
+      <c r="C215" s="10"/>
+      <c r="D215" s="10"/>
+      <c r="E215" s="10"/>
     </row>
     <row r="216" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
@@ -10038,16 +10082,16 @@
       <c r="A218" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="B218" s="5" t="s">
+      <c r="B218" s="9" t="s">
         <v>835</v>
       </c>
-      <c r="C218" s="5" t="s">
+      <c r="C218" s="9" t="s">
         <v>836</v>
       </c>
-      <c r="D218" s="5" t="s">
+      <c r="D218" s="9" t="s">
         <v>837</v>
       </c>
-      <c r="E218" s="5" t="s">
+      <c r="E218" s="9" t="s">
         <v>838</v>
       </c>
     </row>
@@ -10055,10 +10099,10 @@
       <c r="A219" s="4" t="s">
         <v>834</v>
       </c>
-      <c r="B219" s="6"/>
-      <c r="C219" s="6"/>
-      <c r="D219" s="6"/>
-      <c r="E219" s="6"/>
+      <c r="B219" s="10"/>
+      <c r="C219" s="10"/>
+      <c r="D219" s="10"/>
+      <c r="E219" s="10"/>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
@@ -10288,16 +10332,16 @@
       <c r="A234" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="B234" s="5" t="s">
+      <c r="B234" s="9" t="s">
         <v>835</v>
       </c>
-      <c r="C234" s="5" t="s">
+      <c r="C234" s="9" t="s">
         <v>836</v>
       </c>
-      <c r="D234" s="5" t="s">
+      <c r="D234" s="9" t="s">
         <v>837</v>
       </c>
-      <c r="E234" s="5" t="s">
+      <c r="E234" s="9" t="s">
         <v>838</v>
       </c>
     </row>
@@ -10305,10 +10349,10 @@
       <c r="A235" s="4" t="s">
         <v>834</v>
       </c>
-      <c r="B235" s="6"/>
-      <c r="C235" s="6"/>
-      <c r="D235" s="6"/>
-      <c r="E235" s="6"/>
+      <c r="B235" s="10"/>
+      <c r="C235" s="10"/>
+      <c r="D235" s="10"/>
+      <c r="E235" s="10"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
@@ -10536,16 +10580,16 @@
       <c r="A250" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="B250" s="5" t="s">
+      <c r="B250" s="9" t="s">
         <v>677</v>
       </c>
-      <c r="C250" s="5" t="s">
+      <c r="C250" s="9" t="s">
         <v>678</v>
       </c>
-      <c r="D250" s="5" t="s">
+      <c r="D250" s="9" t="s">
         <v>679</v>
       </c>
-      <c r="E250" s="5" t="s">
+      <c r="E250" s="9" t="s">
         <v>680</v>
       </c>
     </row>
@@ -10553,10 +10597,10 @@
       <c r="A251" s="4" t="s">
         <v>676</v>
       </c>
-      <c r="B251" s="6"/>
-      <c r="C251" s="6"/>
-      <c r="D251" s="6"/>
-      <c r="E251" s="6"/>
+      <c r="B251" s="10"/>
+      <c r="C251" s="10"/>
+      <c r="D251" s="10"/>
+      <c r="E251" s="10"/>
     </row>
     <row r="252" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
@@ -11292,16 +11336,16 @@
       <c r="A298" s="3" t="s">
         <v>1157</v>
       </c>
-      <c r="B298" s="5" t="s">
+      <c r="B298" s="9" t="s">
         <v>1159</v>
       </c>
-      <c r="C298" s="5" t="s">
+      <c r="C298" s="9" t="s">
         <v>1160</v>
       </c>
-      <c r="D298" s="5" t="s">
+      <c r="D298" s="9" t="s">
         <v>1161</v>
       </c>
-      <c r="E298" s="5" t="s">
+      <c r="E298" s="9" t="s">
         <v>1162</v>
       </c>
     </row>
@@ -11309,10 +11353,10 @@
       <c r="A299" s="4" t="s">
         <v>1158</v>
       </c>
-      <c r="B299" s="6"/>
-      <c r="C299" s="6"/>
-      <c r="D299" s="6"/>
-      <c r="E299" s="6"/>
+      <c r="B299" s="10"/>
+      <c r="C299" s="10"/>
+      <c r="D299" s="10"/>
+      <c r="E299" s="10"/>
     </row>
     <row r="300" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
@@ -11427,16 +11471,16 @@
       <c r="A307" s="3" t="s">
         <v>1191</v>
       </c>
-      <c r="B307" s="5" t="s">
+      <c r="B307" s="9" t="s">
         <v>1193</v>
       </c>
-      <c r="C307" s="5" t="s">
+      <c r="C307" s="9" t="s">
         <v>1194</v>
       </c>
-      <c r="D307" s="5" t="s">
+      <c r="D307" s="9" t="s">
         <v>1195</v>
       </c>
-      <c r="E307" s="5" t="s">
+      <c r="E307" s="9" t="s">
         <v>1196</v>
       </c>
     </row>
@@ -11444,10 +11488,10 @@
       <c r="A308" s="4" t="s">
         <v>1192</v>
       </c>
-      <c r="B308" s="6"/>
-      <c r="C308" s="6"/>
-      <c r="D308" s="6"/>
-      <c r="E308" s="6"/>
+      <c r="B308" s="10"/>
+      <c r="C308" s="10"/>
+      <c r="D308" s="10"/>
+      <c r="E308" s="10"/>
     </row>
     <row r="309" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
@@ -11500,16 +11544,16 @@
       <c r="A312" s="3" t="s">
         <v>1209</v>
       </c>
-      <c r="B312" s="5" t="s">
+      <c r="B312" s="9" t="s">
         <v>1211</v>
       </c>
-      <c r="C312" s="5" t="s">
+      <c r="C312" s="9" t="s">
         <v>1212</v>
       </c>
-      <c r="D312" s="5" t="s">
+      <c r="D312" s="9" t="s">
         <v>1213</v>
       </c>
-      <c r="E312" s="5" t="s">
+      <c r="E312" s="9" t="s">
         <v>1214</v>
       </c>
     </row>
@@ -11517,10 +11561,10 @@
       <c r="A313" s="4" t="s">
         <v>1210</v>
       </c>
-      <c r="B313" s="6"/>
-      <c r="C313" s="6"/>
-      <c r="D313" s="6"/>
-      <c r="E313" s="6"/>
+      <c r="B313" s="10"/>
+      <c r="C313" s="10"/>
+      <c r="D313" s="10"/>
+      <c r="E313" s="10"/>
     </row>
     <row r="314" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
@@ -11631,16 +11675,16 @@
       <c r="A321" s="3" t="s">
         <v>1157</v>
       </c>
-      <c r="B321" s="5" t="s">
+      <c r="B321" s="9" t="s">
         <v>1159</v>
       </c>
-      <c r="C321" s="5" t="s">
+      <c r="C321" s="9" t="s">
         <v>1160</v>
       </c>
-      <c r="D321" s="5" t="s">
+      <c r="D321" s="9" t="s">
         <v>1161</v>
       </c>
-      <c r="E321" s="5" t="s">
+      <c r="E321" s="9" t="s">
         <v>1162</v>
       </c>
     </row>
@@ -11648,10 +11692,10 @@
       <c r="A322" s="4" t="s">
         <v>1158</v>
       </c>
-      <c r="B322" s="6"/>
-      <c r="C322" s="6"/>
-      <c r="D322" s="6"/>
-      <c r="E322" s="6"/>
+      <c r="B322" s="10"/>
+      <c r="C322" s="10"/>
+      <c r="D322" s="10"/>
+      <c r="E322" s="10"/>
     </row>
     <row r="323" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
@@ -11798,16 +11842,16 @@
       <c r="A332" s="3" t="s">
         <v>1191</v>
       </c>
-      <c r="B332" s="5" t="s">
+      <c r="B332" s="9" t="s">
         <v>1193</v>
       </c>
-      <c r="C332" s="5" t="s">
+      <c r="C332" s="9" t="s">
         <v>1194</v>
       </c>
-      <c r="D332" s="5" t="s">
+      <c r="D332" s="9" t="s">
         <v>1195</v>
       </c>
-      <c r="E332" s="5" t="s">
+      <c r="E332" s="9" t="s">
         <v>1196</v>
       </c>
     </row>
@@ -11815,25 +11859,25 @@
       <c r="A333" s="4" t="s">
         <v>1192</v>
       </c>
-      <c r="B333" s="6"/>
-      <c r="C333" s="6"/>
-      <c r="D333" s="6"/>
-      <c r="E333" s="6"/>
+      <c r="B333" s="10"/>
+      <c r="C333" s="10"/>
+      <c r="D333" s="10"/>
+      <c r="E333" s="10"/>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="3" t="s">
         <v>1209</v>
       </c>
-      <c r="B334" s="5" t="s">
+      <c r="B334" s="9" t="s">
         <v>1211</v>
       </c>
-      <c r="C334" s="5" t="s">
+      <c r="C334" s="9" t="s">
         <v>1212</v>
       </c>
-      <c r="D334" s="5" t="s">
+      <c r="D334" s="9" t="s">
         <v>1213</v>
       </c>
-      <c r="E334" s="5" t="s">
+      <c r="E334" s="9" t="s">
         <v>1214</v>
       </c>
     </row>
@@ -11841,10 +11885,10 @@
       <c r="A335" s="4" t="s">
         <v>1210</v>
       </c>
-      <c r="B335" s="6"/>
-      <c r="C335" s="6"/>
-      <c r="D335" s="6"/>
-      <c r="E335" s="6"/>
+      <c r="B335" s="10"/>
+      <c r="C335" s="10"/>
+      <c r="D335" s="10"/>
+      <c r="E335" s="10"/>
     </row>
     <row r="336" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
@@ -11925,16 +11969,16 @@
       <c r="A341" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B341" s="5" t="s">
+      <c r="B341" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="C341" s="5" t="s">
+      <c r="C341" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="D341" s="5" t="s">
+      <c r="D341" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="E341" s="5" t="s">
+      <c r="E341" s="9" t="s">
         <v>298</v>
       </c>
     </row>
@@ -11942,10 +11986,10 @@
       <c r="A342" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B342" s="6"/>
-      <c r="C342" s="6"/>
-      <c r="D342" s="6"/>
-      <c r="E342" s="6"/>
+      <c r="B342" s="10"/>
+      <c r="C342" s="10"/>
+      <c r="D342" s="10"/>
+      <c r="E342" s="10"/>
     </row>
     <row r="343" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
@@ -12203,16 +12247,16 @@
       <c r="A359" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="B359" s="5" t="s">
+      <c r="B359" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="C359" s="5" t="s">
+      <c r="C359" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="D359" s="5" t="s">
+      <c r="D359" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="E359" s="5" t="s">
+      <c r="E359" s="9" t="s">
         <v>528</v>
       </c>
     </row>
@@ -12220,10 +12264,10 @@
       <c r="A360" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="B360" s="6"/>
-      <c r="C360" s="6"/>
-      <c r="D360" s="6"/>
-      <c r="E360" s="6"/>
+      <c r="B360" s="10"/>
+      <c r="C360" s="10"/>
+      <c r="D360" s="10"/>
+      <c r="E360" s="10"/>
     </row>
     <row r="361" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
@@ -12699,16 +12743,16 @@
       <c r="A391" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="B391" s="5" t="s">
+      <c r="B391" s="9" t="s">
         <v>594</v>
       </c>
-      <c r="C391" s="5" t="s">
+      <c r="C391" s="9" t="s">
         <v>595</v>
       </c>
-      <c r="D391" s="5" t="s">
+      <c r="D391" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="E391" s="5" t="s">
+      <c r="E391" s="9" t="s">
         <v>597</v>
       </c>
     </row>
@@ -12716,10 +12760,10 @@
       <c r="A392" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="B392" s="6"/>
-      <c r="C392" s="6"/>
-      <c r="D392" s="6"/>
-      <c r="E392" s="6"/>
+      <c r="B392" s="10"/>
+      <c r="C392" s="10"/>
+      <c r="D392" s="10"/>
+      <c r="E392" s="10"/>
     </row>
     <row r="393" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
@@ -12992,16 +13036,16 @@
       <c r="A410" s="3" t="s">
         <v>1569</v>
       </c>
-      <c r="B410" s="5" t="s">
+      <c r="B410" s="9" t="s">
         <v>1571</v>
       </c>
-      <c r="C410" s="5" t="s">
+      <c r="C410" s="9" t="s">
         <v>1572</v>
       </c>
-      <c r="D410" s="5" t="s">
+      <c r="D410" s="9" t="s">
         <v>1573</v>
       </c>
-      <c r="E410" s="5" t="s">
+      <c r="E410" s="9" t="s">
         <v>1574</v>
       </c>
     </row>
@@ -13009,25 +13053,25 @@
       <c r="A411" s="4" t="s">
         <v>1570</v>
       </c>
-      <c r="B411" s="6"/>
-      <c r="C411" s="6"/>
-      <c r="D411" s="6"/>
-      <c r="E411" s="6"/>
+      <c r="B411" s="10"/>
+      <c r="C411" s="10"/>
+      <c r="D411" s="10"/>
+      <c r="E411" s="10"/>
     </row>
     <row r="412" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A412" s="3" t="s">
         <v>1569</v>
       </c>
-      <c r="B412" s="5" t="s">
+      <c r="B412" s="9" t="s">
         <v>1571</v>
       </c>
-      <c r="C412" s="5" t="s">
+      <c r="C412" s="9" t="s">
         <v>1572</v>
       </c>
-      <c r="D412" s="5" t="s">
+      <c r="D412" s="9" t="s">
         <v>1573</v>
       </c>
-      <c r="E412" s="5" t="s">
+      <c r="E412" s="9" t="s">
         <v>1574</v>
       </c>
     </row>
@@ -13035,10 +13079,10 @@
       <c r="A413" s="4" t="s">
         <v>1570</v>
       </c>
-      <c r="B413" s="6"/>
-      <c r="C413" s="6"/>
-      <c r="D413" s="6"/>
-      <c r="E413" s="6"/>
+      <c r="B413" s="10"/>
+      <c r="C413" s="10"/>
+      <c r="D413" s="10"/>
+      <c r="E413" s="10"/>
     </row>
     <row r="414" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
@@ -13414,16 +13458,16 @@
       <c r="A438" s="3" t="s">
         <v>1673</v>
       </c>
-      <c r="B438" s="5" t="s">
+      <c r="B438" s="9" t="s">
         <v>1675</v>
       </c>
-      <c r="C438" s="5" t="s">
+      <c r="C438" s="9" t="s">
         <v>1676</v>
       </c>
-      <c r="D438" s="5" t="s">
+      <c r="D438" s="9" t="s">
         <v>1677</v>
       </c>
-      <c r="E438" s="5" t="s">
+      <c r="E438" s="9" t="s">
         <v>1678</v>
       </c>
     </row>
@@ -13431,25 +13475,25 @@
       <c r="A439" s="4" t="s">
         <v>1674</v>
       </c>
-      <c r="B439" s="6"/>
-      <c r="C439" s="6"/>
-      <c r="D439" s="6"/>
-      <c r="E439" s="6"/>
+      <c r="B439" s="10"/>
+      <c r="C439" s="10"/>
+      <c r="D439" s="10"/>
+      <c r="E439" s="10"/>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A440" s="3" t="s">
         <v>1673</v>
       </c>
-      <c r="B440" s="5" t="s">
+      <c r="B440" s="9" t="s">
         <v>1675</v>
       </c>
-      <c r="C440" s="5" t="s">
+      <c r="C440" s="9" t="s">
         <v>1676</v>
       </c>
-      <c r="D440" s="5" t="s">
+      <c r="D440" s="9" t="s">
         <v>1677</v>
       </c>
-      <c r="E440" s="5" t="s">
+      <c r="E440" s="9" t="s">
         <v>1678</v>
       </c>
     </row>
@@ -13457,10 +13501,10 @@
       <c r="A441" s="4" t="s">
         <v>1674</v>
       </c>
-      <c r="B441" s="6"/>
-      <c r="C441" s="6"/>
-      <c r="D441" s="6"/>
-      <c r="E441" s="6"/>
+      <c r="B441" s="10"/>
+      <c r="C441" s="10"/>
+      <c r="D441" s="10"/>
+      <c r="E441" s="10"/>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
@@ -13701,7 +13745,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="457" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
         <v>1745</v>
       </c>
@@ -13709,29 +13753,29 @@
         <v>1746</v>
       </c>
       <c r="C457" s="2" t="s">
+        <v>2102</v>
+      </c>
+      <c r="D457" s="2" t="s">
+        <v>2103</v>
+      </c>
+      <c r="E457" s="2" t="s">
         <v>1747</v>
-      </c>
-      <c r="D457" s="2" t="s">
-        <v>1748</v>
-      </c>
-      <c r="E457" s="2" t="s">
-        <v>1749</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A458" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B458" s="5" t="s">
+      <c r="B458" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C458" s="5" t="s">
+      <c r="C458" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D458" s="5" t="s">
+      <c r="D458" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E458" s="5" t="s">
+      <c r="E458" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -13739,426 +13783,426 @@
       <c r="A459" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B459" s="6"/>
-      <c r="C459" s="6"/>
-      <c r="D459" s="6"/>
-      <c r="E459" s="6"/>
+      <c r="B459" s="10"/>
+      <c r="C459" s="10"/>
+      <c r="D459" s="10"/>
+      <c r="E459" s="10"/>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B460" s="2" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C460" s="2" t="s">
         <v>1750</v>
       </c>
-      <c r="B460" s="2" t="s">
+      <c r="D460" s="2" t="s">
         <v>1751</v>
       </c>
-      <c r="C460" s="2" t="s">
+      <c r="E460" s="2" t="s">
         <v>1752</v>
-      </c>
-      <c r="D460" s="2" t="s">
-        <v>1753</v>
-      </c>
-      <c r="E460" s="2" t="s">
-        <v>1754</v>
       </c>
     </row>
     <row r="461" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="B461" s="2"/>
       <c r="C461" s="2" t="s">
+        <v>1754</v>
+      </c>
+      <c r="D461" s="2" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E461" s="2" t="s">
         <v>1756</v>
-      </c>
-      <c r="D461" s="2" t="s">
-        <v>1757</v>
-      </c>
-      <c r="E461" s="2" t="s">
-        <v>1758</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B462" s="2" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C462" s="2" t="s">
         <v>1759</v>
       </c>
-      <c r="B462" s="2" t="s">
+      <c r="D462" s="2" t="s">
         <v>1760</v>
       </c>
-      <c r="C462" s="2" t="s">
+      <c r="E462" s="2" t="s">
         <v>1761</v>
-      </c>
-      <c r="D462" s="2" t="s">
-        <v>1762</v>
-      </c>
-      <c r="E462" s="2" t="s">
-        <v>1763</v>
       </c>
     </row>
     <row r="463" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="B463" s="2"/>
       <c r="C463" s="2" t="s">
+        <v>1763</v>
+      </c>
+      <c r="D463" s="2" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E463" s="2" t="s">
         <v>1765</v>
-      </c>
-      <c r="D463" s="2" t="s">
-        <v>1766</v>
-      </c>
-      <c r="E463" s="2" t="s">
-        <v>1767</v>
       </c>
     </row>
     <row r="464" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
-        <v>1768</v>
+        <v>1766</v>
       </c>
       <c r="B464" s="2"/>
       <c r="C464" s="2" t="s">
+        <v>1767</v>
+      </c>
+      <c r="D464" s="2" t="s">
+        <v>1768</v>
+      </c>
+      <c r="E464" s="2" t="s">
         <v>1769</v>
-      </c>
-      <c r="D464" s="2" t="s">
-        <v>1770</v>
-      </c>
-      <c r="E464" s="2" t="s">
-        <v>1771</v>
       </c>
     </row>
     <row r="465" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B465" s="2" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C465" s="2" t="s">
         <v>1772</v>
       </c>
-      <c r="B465" s="2" t="s">
+      <c r="D465" s="2" t="s">
         <v>1773</v>
       </c>
-      <c r="C465" s="2" t="s">
+      <c r="E465" s="2" t="s">
         <v>1774</v>
-      </c>
-      <c r="D465" s="2" t="s">
-        <v>1775</v>
-      </c>
-      <c r="E465" s="2" t="s">
-        <v>1776</v>
       </c>
     </row>
     <row r="466" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
-        <v>1777</v>
+        <v>1775</v>
       </c>
       <c r="B466" s="2"/>
       <c r="C466" s="2" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D466" s="2" t="s">
+        <v>1777</v>
+      </c>
+      <c r="E466" s="2" t="s">
         <v>1778</v>
-      </c>
-      <c r="D466" s="2" t="s">
-        <v>1779</v>
-      </c>
-      <c r="E466" s="2" t="s">
-        <v>1780</v>
       </c>
     </row>
     <row r="467" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B467" s="2" t="s">
+        <v>1780</v>
+      </c>
+      <c r="C467" s="2" t="s">
         <v>1781</v>
       </c>
-      <c r="B467" s="2" t="s">
+      <c r="D467" s="2" t="s">
         <v>1782</v>
       </c>
-      <c r="C467" s="2" t="s">
+      <c r="E467" s="2" t="s">
         <v>1783</v>
-      </c>
-      <c r="D467" s="2" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E467" s="2" t="s">
-        <v>1785</v>
       </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
       <c r="B468" s="2"/>
       <c r="C468" s="2" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="D468" s="2" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
       <c r="E468" s="2" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
       <c r="B469" s="2"/>
       <c r="C469" s="2" t="s">
+        <v>1788</v>
+      </c>
+      <c r="D469" s="2" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E469" s="2" t="s">
         <v>1790</v>
-      </c>
-      <c r="D469" s="2" t="s">
-        <v>1791</v>
-      </c>
-      <c r="E469" s="2" t="s">
-        <v>1792</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B470" s="2" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C470" s="2" t="s">
         <v>1793</v>
       </c>
-      <c r="B470" s="2" t="s">
+      <c r="D470" s="2" t="s">
         <v>1794</v>
       </c>
-      <c r="C470" s="2" t="s">
-        <v>1795</v>
-      </c>
-      <c r="D470" s="2" t="s">
-        <v>1796</v>
-      </c>
       <c r="E470" s="2" t="s">
-        <v>1795</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B471" s="2" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C471" s="2" t="s">
         <v>1797</v>
       </c>
-      <c r="B471" s="2" t="s">
+      <c r="D471" s="2" t="s">
         <v>1798</v>
       </c>
-      <c r="C471" s="2" t="s">
+      <c r="E471" s="2" t="s">
         <v>1799</v>
-      </c>
-      <c r="D471" s="2" t="s">
-        <v>1800</v>
-      </c>
-      <c r="E471" s="2" t="s">
-        <v>1801</v>
       </c>
     </row>
     <row r="472" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A472" s="2" t="s">
-        <v>1802</v>
+        <v>1800</v>
       </c>
       <c r="B472" s="2"/>
       <c r="C472" s="2" t="s">
+        <v>1801</v>
+      </c>
+      <c r="D472" s="2" t="s">
+        <v>1802</v>
+      </c>
+      <c r="E472" s="2" t="s">
         <v>1803</v>
-      </c>
-      <c r="D472" s="2" t="s">
-        <v>1804</v>
-      </c>
-      <c r="E472" s="2" t="s">
-        <v>1805</v>
       </c>
     </row>
     <row r="473" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="B473" s="2"/>
       <c r="C473" s="2" t="s">
+        <v>1805</v>
+      </c>
+      <c r="D473" s="2" t="s">
+        <v>1806</v>
+      </c>
+      <c r="E473" s="2" t="s">
         <v>1807</v>
-      </c>
-      <c r="D473" s="2" t="s">
-        <v>1808</v>
-      </c>
-      <c r="E473" s="2" t="s">
-        <v>1809</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A474" s="2" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B474" s="2" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C474" s="2" t="s">
         <v>1810</v>
       </c>
-      <c r="B474" s="2" t="s">
+      <c r="D474" s="2" t="s">
         <v>1811</v>
       </c>
-      <c r="C474" s="2" t="s">
+      <c r="E474" s="2" t="s">
         <v>1812</v>
-      </c>
-      <c r="D474" s="2" t="s">
-        <v>1813</v>
-      </c>
-      <c r="E474" s="2" t="s">
-        <v>1814</v>
       </c>
     </row>
     <row r="475" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
-        <v>1815</v>
+        <v>1813</v>
       </c>
       <c r="B475" s="2"/>
       <c r="C475" s="2" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D475" s="2" t="s">
+        <v>1815</v>
+      </c>
+      <c r="E475" s="2" t="s">
         <v>1816</v>
-      </c>
-      <c r="D475" s="2" t="s">
-        <v>1817</v>
-      </c>
-      <c r="E475" s="2" t="s">
-        <v>1818</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A476" s="2" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B476" s="2" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C476" s="2" t="s">
         <v>1819</v>
       </c>
-      <c r="B476" s="2" t="s">
+      <c r="D476" s="2" t="s">
         <v>1820</v>
       </c>
-      <c r="C476" s="2" t="s">
-        <v>1821</v>
-      </c>
-      <c r="D476" s="2" t="s">
-        <v>1822</v>
-      </c>
       <c r="E476" s="2" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B477" s="2" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C477" s="2" t="s">
         <v>1823</v>
       </c>
-      <c r="B477" s="2" t="s">
+      <c r="D477" s="2" t="s">
         <v>1824</v>
       </c>
-      <c r="C477" s="2" t="s">
+      <c r="E477" s="2" t="s">
         <v>1825</v>
-      </c>
-      <c r="D477" s="2" t="s">
-        <v>1826</v>
-      </c>
-      <c r="E477" s="2" t="s">
-        <v>1827</v>
       </c>
     </row>
     <row r="478" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B478" s="2" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C478" s="2" t="s">
         <v>1828</v>
       </c>
-      <c r="B478" s="2" t="s">
+      <c r="D478" s="2" t="s">
         <v>1829</v>
       </c>
-      <c r="C478" s="2" t="s">
+      <c r="E478" s="2" t="s">
         <v>1830</v>
-      </c>
-      <c r="D478" s="2" t="s">
-        <v>1831</v>
-      </c>
-      <c r="E478" s="2" t="s">
-        <v>1832</v>
       </c>
     </row>
     <row r="479" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="B479" s="2"/>
       <c r="C479" s="2" t="s">
+        <v>1832</v>
+      </c>
+      <c r="D479" s="2" t="s">
+        <v>1833</v>
+      </c>
+      <c r="E479" s="2" t="s">
         <v>1834</v>
-      </c>
-      <c r="D479" s="2" t="s">
-        <v>1835</v>
-      </c>
-      <c r="E479" s="2" t="s">
-        <v>1836</v>
       </c>
     </row>
     <row r="480" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A480" s="2" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="B480" s="2"/>
       <c r="C480" s="2" t="s">
+        <v>1836</v>
+      </c>
+      <c r="D480" s="2" t="s">
+        <v>1837</v>
+      </c>
+      <c r="E480" s="2" t="s">
         <v>1838</v>
-      </c>
-      <c r="D480" s="2" t="s">
-        <v>1839</v>
-      </c>
-      <c r="E480" s="2" t="s">
-        <v>1840</v>
       </c>
     </row>
     <row r="481" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
       <c r="B481" s="2"/>
       <c r="C481" s="2" t="s">
+        <v>1840</v>
+      </c>
+      <c r="D481" s="2" t="s">
+        <v>1841</v>
+      </c>
+      <c r="E481" s="2" t="s">
         <v>1842</v>
-      </c>
-      <c r="D481" s="2" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E481" s="2" t="s">
-        <v>1844</v>
       </c>
     </row>
     <row r="482" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A482" s="2" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B482" s="2" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C482" s="2" t="s">
         <v>1845</v>
       </c>
-      <c r="B482" s="2" t="s">
+      <c r="D482" s="2" t="s">
         <v>1846</v>
       </c>
-      <c r="C482" s="2" t="s">
+      <c r="E482" s="2" t="s">
         <v>1847</v>
-      </c>
-      <c r="D482" s="2" t="s">
-        <v>1848</v>
-      </c>
-      <c r="E482" s="2" t="s">
-        <v>1849</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B483" s="2" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C483" s="2" t="s">
         <v>1850</v>
       </c>
-      <c r="B483" s="2" t="s">
+      <c r="D483" s="2" t="s">
         <v>1851</v>
       </c>
-      <c r="C483" s="2" t="s">
-        <v>1852</v>
-      </c>
-      <c r="D483" s="2" t="s">
-        <v>1853</v>
-      </c>
       <c r="E483" s="2" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B484" s="2" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C484" s="2" t="s">
         <v>1854</v>
       </c>
-      <c r="B484" s="2" t="s">
+      <c r="D484" s="2" t="s">
         <v>1855</v>
       </c>
-      <c r="C484" s="2" t="s">
+      <c r="E484" s="2" t="s">
         <v>1856</v>
-      </c>
-      <c r="D484" s="2" t="s">
-        <v>1857</v>
-      </c>
-      <c r="E484" s="2" t="s">
-        <v>1858</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A485" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B485" s="5" t="s">
+      <c r="B485" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C485" s="5" t="s">
+      <c r="C485" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="D485" s="5" t="s">
+      <c r="D485" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="E485" s="5" t="s">
+      <c r="E485" s="9" t="s">
         <v>261</v>
       </c>
     </row>
@@ -14166,623 +14210,623 @@
       <c r="A486" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B486" s="6"/>
-      <c r="C486" s="6"/>
-      <c r="D486" s="6"/>
-      <c r="E486" s="6"/>
+      <c r="B486" s="10"/>
+      <c r="C486" s="10"/>
+      <c r="D486" s="10"/>
+      <c r="E486" s="10"/>
     </row>
     <row r="487" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
-        <v>1859</v>
+        <v>1857</v>
       </c>
       <c r="B487" s="2"/>
       <c r="C487" s="2" t="s">
+        <v>1858</v>
+      </c>
+      <c r="D487" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="E487" s="2" t="s">
         <v>1860</v>
-      </c>
-      <c r="D487" s="2" t="s">
-        <v>1861</v>
-      </c>
-      <c r="E487" s="2" t="s">
-        <v>1862</v>
       </c>
     </row>
     <row r="488" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B488" s="2" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C488" s="2" t="s">
         <v>1863</v>
       </c>
-      <c r="B488" s="2" t="s">
+      <c r="D488" s="2" t="s">
         <v>1864</v>
       </c>
-      <c r="C488" s="2" t="s">
+      <c r="E488" s="2" t="s">
         <v>1865</v>
-      </c>
-      <c r="D488" s="2" t="s">
-        <v>1866</v>
-      </c>
-      <c r="E488" s="2" t="s">
-        <v>1867</v>
       </c>
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
       <c r="B489" s="2"/>
       <c r="C489" s="2" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="D489" s="2" t="s">
+        <v>1866</v>
+      </c>
+      <c r="E489" s="2" t="s">
         <v>1868</v>
-      </c>
-      <c r="E489" s="2" t="s">
-        <v>1870</v>
       </c>
     </row>
     <row r="490" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="B490" s="2"/>
       <c r="C490" s="2" t="s">
+        <v>1870</v>
+      </c>
+      <c r="D490" s="2" t="s">
+        <v>1871</v>
+      </c>
+      <c r="E490" s="2" t="s">
         <v>1872</v>
-      </c>
-      <c r="D490" s="2" t="s">
-        <v>1873</v>
-      </c>
-      <c r="E490" s="2" t="s">
-        <v>1874</v>
       </c>
     </row>
     <row r="491" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="B491" s="2"/>
       <c r="C491" s="2" t="s">
+        <v>1874</v>
+      </c>
+      <c r="D491" s="2" t="s">
+        <v>1875</v>
+      </c>
+      <c r="E491" s="2" t="s">
         <v>1876</v>
-      </c>
-      <c r="D491" s="2" t="s">
-        <v>1877</v>
-      </c>
-      <c r="E491" s="2" t="s">
-        <v>1878</v>
       </c>
     </row>
     <row r="492" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="B492" s="2"/>
       <c r="C492" s="2" t="s">
+        <v>1878</v>
+      </c>
+      <c r="D492" s="2" t="s">
+        <v>1879</v>
+      </c>
+      <c r="E492" s="2" t="s">
         <v>1880</v>
-      </c>
-      <c r="D492" s="2" t="s">
-        <v>1881</v>
-      </c>
-      <c r="E492" s="2" t="s">
-        <v>1882</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A493" s="2" t="s">
-        <v>1883</v>
+        <v>1881</v>
       </c>
       <c r="B493" s="2"/>
       <c r="C493" s="2" t="s">
+        <v>1882</v>
+      </c>
+      <c r="D493" s="2" t="s">
+        <v>1883</v>
+      </c>
+      <c r="E493" s="2" t="s">
         <v>1884</v>
-      </c>
-      <c r="D493" s="2" t="s">
-        <v>1885</v>
-      </c>
-      <c r="E493" s="2" t="s">
-        <v>1886</v>
       </c>
     </row>
     <row r="494" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A494" s="2" t="s">
-        <v>1887</v>
+        <v>1885</v>
       </c>
       <c r="B494" s="2"/>
       <c r="C494" s="2" t="s">
+        <v>1886</v>
+      </c>
+      <c r="D494" s="2" t="s">
+        <v>1887</v>
+      </c>
+      <c r="E494" s="2" t="s">
         <v>1888</v>
-      </c>
-      <c r="D494" s="2" t="s">
-        <v>1889</v>
-      </c>
-      <c r="E494" s="2" t="s">
-        <v>1890</v>
       </c>
     </row>
     <row r="495" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A495" s="2" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B495" s="2" t="s">
+        <v>1890</v>
+      </c>
+      <c r="C495" s="2" t="s">
         <v>1891</v>
       </c>
-      <c r="B495" s="2" t="s">
+      <c r="D495" s="2" t="s">
         <v>1892</v>
       </c>
-      <c r="C495" s="2" t="s">
+      <c r="E495" s="2" t="s">
         <v>1893</v>
-      </c>
-      <c r="D495" s="2" t="s">
-        <v>1894</v>
-      </c>
-      <c r="E495" s="2" t="s">
-        <v>1895</v>
       </c>
     </row>
     <row r="496" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A496" s="2" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
       <c r="B496" s="2"/>
       <c r="C496" s="2" t="s">
+        <v>1895</v>
+      </c>
+      <c r="D496" s="2" t="s">
+        <v>1896</v>
+      </c>
+      <c r="E496" s="2" t="s">
         <v>1897</v>
-      </c>
-      <c r="D496" s="2" t="s">
-        <v>1898</v>
-      </c>
-      <c r="E496" s="2" t="s">
-        <v>1899</v>
       </c>
     </row>
     <row r="497" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A497" s="2" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
       <c r="B497" s="2"/>
       <c r="C497" s="2" t="s">
+        <v>1899</v>
+      </c>
+      <c r="D497" s="2" t="s">
+        <v>1900</v>
+      </c>
+      <c r="E497" s="2" t="s">
         <v>1901</v>
-      </c>
-      <c r="D497" s="2" t="s">
-        <v>1902</v>
-      </c>
-      <c r="E497" s="2" t="s">
-        <v>1903</v>
       </c>
     </row>
     <row r="498" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A498" s="2" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B498" s="2" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C498" s="2" t="s">
         <v>1904</v>
       </c>
-      <c r="B498" s="2" t="s">
+      <c r="D498" s="2" t="s">
         <v>1905</v>
       </c>
-      <c r="C498" s="2" t="s">
+      <c r="E498" s="2" t="s">
         <v>1906</v>
-      </c>
-      <c r="D498" s="2" t="s">
-        <v>1907</v>
-      </c>
-      <c r="E498" s="2" t="s">
-        <v>1908</v>
       </c>
     </row>
     <row r="499" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A499" s="2" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B499" s="2" t="s">
+        <v>1908</v>
+      </c>
+      <c r="C499" s="2" t="s">
         <v>1909</v>
       </c>
-      <c r="B499" s="2" t="s">
+      <c r="D499" s="2" t="s">
         <v>1910</v>
       </c>
-      <c r="C499" s="2" t="s">
+      <c r="E499" s="2" t="s">
         <v>1911</v>
-      </c>
-      <c r="D499" s="2" t="s">
-        <v>1912</v>
-      </c>
-      <c r="E499" s="2" t="s">
-        <v>1913</v>
       </c>
     </row>
     <row r="500" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A500" s="2" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B500" s="2" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C500" s="2" t="s">
         <v>1914</v>
       </c>
-      <c r="B500" s="2" t="s">
+      <c r="D500" s="2" t="s">
         <v>1915</v>
       </c>
-      <c r="C500" s="2" t="s">
+      <c r="E500" s="2" t="s">
         <v>1916</v>
-      </c>
-      <c r="D500" s="2" t="s">
-        <v>1917</v>
-      </c>
-      <c r="E500" s="2" t="s">
-        <v>1918</v>
       </c>
     </row>
     <row r="501" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A501" s="2" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="B501" s="2"/>
       <c r="C501" s="2" t="s">
+        <v>1918</v>
+      </c>
+      <c r="D501" s="2" t="s">
+        <v>1919</v>
+      </c>
+      <c r="E501" s="2" t="s">
         <v>1920</v>
-      </c>
-      <c r="D501" s="2" t="s">
-        <v>1921</v>
-      </c>
-      <c r="E501" s="2" t="s">
-        <v>1922</v>
       </c>
     </row>
     <row r="502" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A502" s="2" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="B502" s="2"/>
       <c r="C502" s="2" t="s">
+        <v>1922</v>
+      </c>
+      <c r="D502" s="2" t="s">
+        <v>1923</v>
+      </c>
+      <c r="E502" s="2" t="s">
         <v>1924</v>
-      </c>
-      <c r="D502" s="2" t="s">
-        <v>1925</v>
-      </c>
-      <c r="E502" s="2" t="s">
-        <v>1926</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A503" s="2" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B503" s="2" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C503" s="2" t="s">
         <v>1927</v>
       </c>
-      <c r="B503" s="2" t="s">
+      <c r="D503" s="2" t="s">
         <v>1928</v>
       </c>
-      <c r="C503" s="2" t="s">
+      <c r="E503" s="2" t="s">
         <v>1929</v>
-      </c>
-      <c r="D503" s="2" t="s">
-        <v>1930</v>
-      </c>
-      <c r="E503" s="2" t="s">
-        <v>1931</v>
       </c>
     </row>
     <row r="504" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A504" s="2" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
       <c r="B504" s="2"/>
       <c r="C504" s="2" t="s">
+        <v>1931</v>
+      </c>
+      <c r="D504" s="2" t="s">
+        <v>1932</v>
+      </c>
+      <c r="E504" s="2" t="s">
         <v>1933</v>
-      </c>
-      <c r="D504" s="2" t="s">
-        <v>1934</v>
-      </c>
-      <c r="E504" s="2" t="s">
-        <v>1935</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A505" s="2" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="B505" s="2"/>
       <c r="C505" s="2" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D505" s="2" t="s">
+        <v>1936</v>
+      </c>
+      <c r="E505" s="2" t="s">
         <v>1937</v>
-      </c>
-      <c r="D505" s="2" t="s">
-        <v>1938</v>
-      </c>
-      <c r="E505" s="2" t="s">
-        <v>1939</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A506" s="2" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>1939</v>
+      </c>
+      <c r="C506" s="2" t="s">
         <v>1940</v>
       </c>
-      <c r="B506" s="2" t="s">
+      <c r="D506" s="2" t="s">
+        <v>1938</v>
+      </c>
+      <c r="E506" s="2" t="s">
         <v>1941</v>
-      </c>
-      <c r="C506" s="2" t="s">
-        <v>1942</v>
-      </c>
-      <c r="D506" s="2" t="s">
-        <v>1940</v>
-      </c>
-      <c r="E506" s="2" t="s">
-        <v>1943</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A507" s="2" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="B507" s="2"/>
       <c r="C507" s="2" t="s">
+        <v>1943</v>
+      </c>
+      <c r="D507" s="2" t="s">
+        <v>1944</v>
+      </c>
+      <c r="E507" s="2" t="s">
         <v>1945</v>
-      </c>
-      <c r="D507" s="2" t="s">
-        <v>1946</v>
-      </c>
-      <c r="E507" s="2" t="s">
-        <v>1947</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A508" s="2" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="B508" s="2"/>
       <c r="C508" s="2" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D508" s="2" t="s">
+        <v>1948</v>
+      </c>
+      <c r="E508" s="2" t="s">
         <v>1949</v>
-      </c>
-      <c r="D508" s="2" t="s">
-        <v>1950</v>
-      </c>
-      <c r="E508" s="2" t="s">
-        <v>1951</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A509" s="2" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="B509" s="2"/>
       <c r="C509" s="2" t="s">
+        <v>1951</v>
+      </c>
+      <c r="D509" s="2" t="s">
+        <v>1952</v>
+      </c>
+      <c r="E509" s="2" t="s">
         <v>1953</v>
-      </c>
-      <c r="D509" s="2" t="s">
-        <v>1954</v>
-      </c>
-      <c r="E509" s="2" t="s">
-        <v>1955</v>
       </c>
     </row>
     <row r="510" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A510" s="2" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B510" s="2" t="s">
+        <v>1955</v>
+      </c>
+      <c r="C510" s="2" t="s">
         <v>1956</v>
       </c>
-      <c r="B510" s="2" t="s">
+      <c r="D510" s="2" t="s">
         <v>1957</v>
       </c>
-      <c r="C510" s="2" t="s">
+      <c r="E510" s="2" t="s">
         <v>1958</v>
-      </c>
-      <c r="D510" s="2" t="s">
-        <v>1959</v>
-      </c>
-      <c r="E510" s="2" t="s">
-        <v>1960</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A511" s="2" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B511" s="2" t="s">
+        <v>1960</v>
+      </c>
+      <c r="C511" s="2" t="s">
         <v>1961</v>
       </c>
-      <c r="B511" s="2" t="s">
+      <c r="D511" s="2" t="s">
         <v>1962</v>
       </c>
-      <c r="C511" s="2" t="s">
+      <c r="E511" s="2" t="s">
         <v>1963</v>
-      </c>
-      <c r="D511" s="2" t="s">
-        <v>1964</v>
-      </c>
-      <c r="E511" s="2" t="s">
-        <v>1965</v>
       </c>
     </row>
     <row r="512" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A512" s="2" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
       <c r="B512" s="2"/>
       <c r="C512" s="2" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D512" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="E512" s="2" t="s">
         <v>1967</v>
-      </c>
-      <c r="D512" s="2" t="s">
-        <v>1968</v>
-      </c>
-      <c r="E512" s="2" t="s">
-        <v>1969</v>
       </c>
     </row>
     <row r="513" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A513" s="2" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="B513" s="2"/>
       <c r="C513" s="2" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D513" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="E513" s="2" t="s">
         <v>1971</v>
-      </c>
-      <c r="D513" s="2" t="s">
-        <v>1972</v>
-      </c>
-      <c r="E513" s="2" t="s">
-        <v>1973</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A514" s="2" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B514" s="2" t="s">
+        <v>1973</v>
+      </c>
+      <c r="C514" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="B514" s="2" t="s">
+      <c r="D514" s="2" t="s">
         <v>1975</v>
       </c>
-      <c r="C514" s="2" t="s">
-        <v>1976</v>
-      </c>
-      <c r="D514" s="2" t="s">
-        <v>1977</v>
-      </c>
       <c r="E514" s="2" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B515" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="C515" s="2" t="s">
         <v>1978</v>
       </c>
-      <c r="B515" s="2" t="s">
+      <c r="D515" s="2" t="s">
         <v>1979</v>
       </c>
-      <c r="C515" s="2" t="s">
+      <c r="E515" s="2" t="s">
         <v>1980</v>
-      </c>
-      <c r="D515" s="2" t="s">
-        <v>1981</v>
-      </c>
-      <c r="E515" s="2" t="s">
-        <v>1982</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A516" s="2" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="B516" s="2"/>
       <c r="C516" s="2" t="s">
+        <v>1982</v>
+      </c>
+      <c r="D516" s="2" t="s">
+        <v>1983</v>
+      </c>
+      <c r="E516" s="2" t="s">
         <v>1984</v>
-      </c>
-      <c r="D516" s="2" t="s">
-        <v>1985</v>
-      </c>
-      <c r="E516" s="2" t="s">
-        <v>1986</v>
       </c>
     </row>
     <row r="517" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B517" s="2" t="s">
+        <v>1986</v>
+      </c>
+      <c r="C517" s="2" t="s">
         <v>1987</v>
       </c>
-      <c r="B517" s="2" t="s">
+      <c r="D517" s="2" t="s">
         <v>1988</v>
       </c>
-      <c r="C517" s="2" t="s">
+      <c r="E517" s="2" t="s">
         <v>1989</v>
-      </c>
-      <c r="D517" s="2" t="s">
-        <v>1990</v>
-      </c>
-      <c r="E517" s="2" t="s">
-        <v>1991</v>
       </c>
     </row>
     <row r="518" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A518" s="2" t="s">
+        <v>1990</v>
+      </c>
+      <c r="B518" s="2" t="s">
+        <v>1991</v>
+      </c>
+      <c r="C518" s="2" t="s">
         <v>1992</v>
       </c>
-      <c r="B518" s="2" t="s">
+      <c r="D518" s="2" t="s">
         <v>1993</v>
       </c>
-      <c r="C518" s="2" t="s">
+      <c r="E518" s="2" t="s">
         <v>1994</v>
-      </c>
-      <c r="D518" s="2" t="s">
-        <v>1995</v>
-      </c>
-      <c r="E518" s="2" t="s">
-        <v>1996</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A519" s="2" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B519" s="2" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C519" s="2" t="s">
         <v>1997</v>
       </c>
-      <c r="B519" s="2" t="s">
+      <c r="D519" s="2" t="s">
         <v>1998</v>
       </c>
-      <c r="C519" s="2" t="s">
-        <v>1999</v>
-      </c>
-      <c r="D519" s="2" t="s">
-        <v>2000</v>
-      </c>
       <c r="E519" s="2" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A520" s="2" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="B520" s="2"/>
       <c r="C520" s="2" t="s">
+        <v>2000</v>
+      </c>
+      <c r="D520" s="2" t="s">
+        <v>2001</v>
+      </c>
+      <c r="E520" s="2" t="s">
         <v>2002</v>
-      </c>
-      <c r="D520" s="2" t="s">
-        <v>2003</v>
-      </c>
-      <c r="E520" s="2" t="s">
-        <v>2004</v>
       </c>
     </row>
     <row r="521" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A521" s="2" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="B521" s="2"/>
       <c r="C521" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="D521" s="2" t="s">
+        <v>2005</v>
+      </c>
+      <c r="E521" s="2" t="s">
         <v>2006</v>
-      </c>
-      <c r="D521" s="2" t="s">
-        <v>2007</v>
-      </c>
-      <c r="E521" s="2" t="s">
-        <v>2008</v>
       </c>
     </row>
     <row r="522" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A522" s="2" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="B522" s="2"/>
       <c r="C522" s="2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="D522" s="2" t="s">
+        <v>2009</v>
+      </c>
+      <c r="E522" s="2" t="s">
         <v>2010</v>
-      </c>
-      <c r="D522" s="2" t="s">
-        <v>2011</v>
-      </c>
-      <c r="E522" s="2" t="s">
-        <v>2012</v>
       </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A523" s="2" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B523" s="2"/>
       <c r="C523" s="2" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D523" s="2" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E523" s="2" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="524" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A524" s="2" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="B524" s="2"/>
       <c r="C524" s="2" t="s">
+        <v>2015</v>
+      </c>
+      <c r="D524" s="2" t="s">
+        <v>2016</v>
+      </c>
+      <c r="E524" s="2" t="s">
         <v>2017</v>
-      </c>
-      <c r="D524" s="2" t="s">
-        <v>2018</v>
-      </c>
-      <c r="E524" s="2" t="s">
-        <v>2019</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A525" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="B525" s="5" t="s">
+      <c r="B525" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="C525" s="5" t="s">
+      <c r="C525" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="D525" s="5" t="s">
+      <c r="D525" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="E525" s="5" t="s">
+      <c r="E525" s="9" t="s">
         <v>459</v>
       </c>
     </row>
@@ -14790,260 +14834,260 @@
       <c r="A526" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="B526" s="6"/>
-      <c r="C526" s="6"/>
-      <c r="D526" s="6"/>
-      <c r="E526" s="6"/>
+      <c r="B526" s="10"/>
+      <c r="C526" s="10"/>
+      <c r="D526" s="10"/>
+      <c r="E526" s="10"/>
     </row>
     <row r="527" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A527" s="2" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="B527" s="2"/>
       <c r="C527" s="2" t="s">
+        <v>2019</v>
+      </c>
+      <c r="D527" s="2" t="s">
+        <v>2020</v>
+      </c>
+      <c r="E527" s="2" t="s">
         <v>2021</v>
-      </c>
-      <c r="D527" s="2" t="s">
-        <v>2022</v>
-      </c>
-      <c r="E527" s="2" t="s">
-        <v>2023</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A528" s="2" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B528" s="2" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C528" s="2" t="s">
         <v>2024</v>
       </c>
-      <c r="B528" s="2" t="s">
+      <c r="D528" s="2" t="s">
         <v>2025</v>
       </c>
-      <c r="C528" s="2" t="s">
+      <c r="E528" s="2" t="s">
         <v>2026</v>
-      </c>
-      <c r="D528" s="2" t="s">
-        <v>2027</v>
-      </c>
-      <c r="E528" s="2" t="s">
-        <v>2028</v>
       </c>
     </row>
     <row r="529" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A529" s="2" t="s">
+        <v>2027</v>
+      </c>
+      <c r="B529" s="2" t="s">
+        <v>2028</v>
+      </c>
+      <c r="C529" s="2" t="s">
         <v>2029</v>
       </c>
-      <c r="B529" s="2" t="s">
+      <c r="D529" s="2" t="s">
         <v>2030</v>
       </c>
-      <c r="C529" s="2" t="s">
+      <c r="E529" s="2" t="s">
         <v>2031</v>
-      </c>
-      <c r="D529" s="2" t="s">
-        <v>2032</v>
-      </c>
-      <c r="E529" s="2" t="s">
-        <v>2033</v>
       </c>
     </row>
     <row r="530" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A530" s="2" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="B530" s="2"/>
       <c r="C530" s="2" t="s">
+        <v>2033</v>
+      </c>
+      <c r="D530" s="2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="E530" s="2" t="s">
         <v>2035</v>
-      </c>
-      <c r="D530" s="2" t="s">
-        <v>2036</v>
-      </c>
-      <c r="E530" s="2" t="s">
-        <v>2037</v>
       </c>
     </row>
     <row r="531" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A531" s="2" t="s">
+        <v>2036</v>
+      </c>
+      <c r="B531" s="2" t="s">
+        <v>2037</v>
+      </c>
+      <c r="C531" s="2" t="s">
         <v>2038</v>
       </c>
-      <c r="B531" s="2" t="s">
+      <c r="D531" s="2" t="s">
         <v>2039</v>
       </c>
-      <c r="C531" s="2" t="s">
+      <c r="E531" s="2" t="s">
         <v>2040</v>
-      </c>
-      <c r="D531" s="2" t="s">
-        <v>2041</v>
-      </c>
-      <c r="E531" s="2" t="s">
-        <v>2042</v>
       </c>
     </row>
     <row r="532" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A532" s="2" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
       <c r="B532" s="2"/>
       <c r="C532" s="2" t="s">
-        <v>2044</v>
+        <v>2042</v>
       </c>
       <c r="D532" s="2" t="s">
+        <v>2041</v>
+      </c>
+      <c r="E532" s="2" t="s">
         <v>2043</v>
-      </c>
-      <c r="E532" s="2" t="s">
-        <v>2045</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A533" s="2" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="B533" s="2"/>
       <c r="C533" s="2" t="s">
+        <v>2045</v>
+      </c>
+      <c r="D533" s="2" t="s">
+        <v>2046</v>
+      </c>
+      <c r="E533" s="2" t="s">
         <v>2047</v>
-      </c>
-      <c r="D533" s="2" t="s">
-        <v>2048</v>
-      </c>
-      <c r="E533" s="2" t="s">
-        <v>2049</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A534" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B534" s="2" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C534" s="2" t="s">
         <v>2050</v>
       </c>
-      <c r="B534" s="2" t="s">
+      <c r="D534" s="2" t="s">
         <v>2051</v>
       </c>
-      <c r="C534" s="2" t="s">
+      <c r="E534" s="2" t="s">
         <v>2052</v>
-      </c>
-      <c r="D534" s="2" t="s">
-        <v>2053</v>
-      </c>
-      <c r="E534" s="2" t="s">
-        <v>2054</v>
       </c>
     </row>
     <row r="535" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A535" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B535" s="2" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C535" s="2" t="s">
         <v>2055</v>
       </c>
-      <c r="B535" s="2" t="s">
+      <c r="D535" s="2" t="s">
         <v>2056</v>
       </c>
-      <c r="C535" s="2" t="s">
+      <c r="E535" s="2" t="s">
         <v>2057</v>
-      </c>
-      <c r="D535" s="2" t="s">
-        <v>2058</v>
-      </c>
-      <c r="E535" s="2" t="s">
-        <v>2059</v>
       </c>
     </row>
     <row r="536" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A536" s="2" t="s">
-        <v>2060</v>
+        <v>2058</v>
       </c>
       <c r="B536" s="2"/>
       <c r="C536" s="2" t="s">
+        <v>2059</v>
+      </c>
+      <c r="D536" s="2" t="s">
+        <v>2060</v>
+      </c>
+      <c r="E536" s="2" t="s">
         <v>2061</v>
-      </c>
-      <c r="D536" s="2" t="s">
-        <v>2062</v>
-      </c>
-      <c r="E536" s="2" t="s">
-        <v>2063</v>
       </c>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A537" s="2" t="s">
-        <v>2064</v>
+        <v>2062</v>
       </c>
       <c r="B537" s="2"/>
       <c r="C537" s="2" t="s">
+        <v>2063</v>
+      </c>
+      <c r="D537" s="2" t="s">
+        <v>2064</v>
+      </c>
+      <c r="E537" s="2" t="s">
         <v>2065</v>
-      </c>
-      <c r="D537" s="2" t="s">
-        <v>2066</v>
-      </c>
-      <c r="E537" s="2" t="s">
-        <v>2067</v>
       </c>
     </row>
     <row r="538" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A538" s="2" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="B538" s="2"/>
       <c r="C538" s="2" t="s">
+        <v>2067</v>
+      </c>
+      <c r="D538" s="2" t="s">
+        <v>2068</v>
+      </c>
+      <c r="E538" s="2" t="s">
         <v>2069</v>
-      </c>
-      <c r="D538" s="2" t="s">
-        <v>2070</v>
-      </c>
-      <c r="E538" s="2" t="s">
-        <v>2071</v>
       </c>
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A539" s="2" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="B539" s="2"/>
       <c r="C539" s="2" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="D539" s="2" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
       <c r="E539" s="2" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="540" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A540" s="2" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="B540" s="2"/>
       <c r="C540" s="2" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
       <c r="D540" s="2" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="E540" s="2"/>
     </row>
     <row r="541" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A541" s="2" t="s">
+        <v>2076</v>
+      </c>
+      <c r="B541" s="2" t="s">
+        <v>2077</v>
+      </c>
+      <c r="C541" s="2" t="s">
         <v>2078</v>
       </c>
-      <c r="B541" s="2" t="s">
+      <c r="D541" s="2" t="s">
         <v>2079</v>
       </c>
-      <c r="C541" s="2" t="s">
+      <c r="E541" s="2" t="s">
         <v>2080</v>
-      </c>
-      <c r="D541" s="2" t="s">
-        <v>2081</v>
-      </c>
-      <c r="E541" s="2" t="s">
-        <v>2082</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A542" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B542" s="5" t="s">
+      <c r="B542" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="C542" s="5" t="s">
+      <c r="C542" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="D542" s="5" t="s">
+      <c r="D542" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="E542" s="5" t="s">
+      <c r="E542" s="9" t="s">
         <v>360</v>
       </c>
     </row>
@@ -15051,87 +15095,109 @@
       <c r="A543" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="B543" s="6"/>
-      <c r="C543" s="6"/>
-      <c r="D543" s="6"/>
-      <c r="E543" s="6"/>
+      <c r="B543" s="10"/>
+      <c r="C543" s="10"/>
+      <c r="D543" s="10"/>
+      <c r="E543" s="10"/>
     </row>
     <row r="544" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A544" s="2" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="B544" s="2"/>
       <c r="C544" s="2" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D544" s="2" t="s">
+        <v>2083</v>
+      </c>
+      <c r="E544" s="2" t="s">
         <v>2084</v>
-      </c>
-      <c r="D544" s="2" t="s">
-        <v>2085</v>
-      </c>
-      <c r="E544" s="2" t="s">
-        <v>2086</v>
       </c>
     </row>
     <row r="545" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A545" s="2" t="s">
+        <v>2085</v>
+      </c>
+      <c r="B545" s="2" t="s">
+        <v>2086</v>
+      </c>
+      <c r="C545" s="2" t="s">
         <v>2087</v>
       </c>
-      <c r="B545" s="2" t="s">
+      <c r="D545" s="2" t="s">
         <v>2088</v>
       </c>
-      <c r="C545" s="2" t="s">
+      <c r="E545" s="2" t="s">
         <v>2089</v>
-      </c>
-      <c r="D545" s="2" t="s">
-        <v>2090</v>
-      </c>
-      <c r="E545" s="2" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="546" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A546" s="2" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="B546" s="2"/>
       <c r="C546" s="2" t="s">
+        <v>2091</v>
+      </c>
+      <c r="D546" s="2" t="s">
+        <v>2092</v>
+      </c>
+      <c r="E546" s="2" t="s">
         <v>2093</v>
-      </c>
-      <c r="D546" s="2" t="s">
-        <v>2094</v>
-      </c>
-      <c r="E546" s="2" t="s">
-        <v>2095</v>
       </c>
     </row>
     <row r="547" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A547" s="2" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
       <c r="B547" s="2"/>
       <c r="C547" s="2" t="s">
+        <v>2095</v>
+      </c>
+      <c r="D547" s="2" t="s">
+        <v>2096</v>
+      </c>
+      <c r="E547" s="2" t="s">
         <v>2097</v>
       </c>
-      <c r="D547" s="2" t="s">
+    </row>
+    <row r="548" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A548" s="5" t="s">
         <v>2098</v>
       </c>
-      <c r="E547" s="2" t="s">
+      <c r="B548" s="5"/>
+      <c r="C548" s="5" t="s">
         <v>2099</v>
       </c>
-    </row>
-    <row r="548" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A548" s="2" t="s">
+      <c r="D548" s="5" t="s">
         <v>2100</v>
       </c>
-      <c r="B548" s="2"/>
-      <c r="C548" s="2" t="s">
+      <c r="E548" s="5" t="s">
         <v>2101</v>
       </c>
-      <c r="D548" s="2" t="s">
-        <v>2102</v>
-      </c>
-      <c r="E548" s="2" t="s">
-        <v>2103</v>
-      </c>
+    </row>
+    <row r="549" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A549" s="6"/>
+      <c r="B549" s="8" t="s">
+        <v>2105</v>
+      </c>
+      <c r="C549" s="7" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D549" s="6"/>
+      <c r="E549" s="6"/>
+    </row>
+    <row r="550" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A550" s="6"/>
+      <c r="B550" s="6" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C550" s="7" t="s">
+        <v>2108</v>
+      </c>
+      <c r="D550" s="6"/>
+      <c r="E550" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="160">

</xml_diff>

<commit_message>
Algerian and Cantonese codes were wrong
</commit_message>
<xml_diff>
--- a/utils/lang_codes.xlsx
+++ b/utils/lang_codes.xlsx
@@ -6341,16 +6341,16 @@
     <t>Greek</t>
   </si>
   <si>
-    <t>zh-yue</t>
-  </si>
-  <si>
     <t>Cantonese</t>
   </si>
   <si>
-    <t>ar-dz</t>
-  </si>
-  <si>
     <t>Algerian</t>
+  </si>
+  <si>
+    <t>zh_yue</t>
+  </si>
+  <si>
+    <t>ar_dz</t>
   </si>
 </sst>
 </file>
@@ -6784,7 +6784,7 @@
   <dimension ref="A1:E550"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
-      <selection activeCell="G552" sqref="G552"/>
+      <selection activeCell="B551" sqref="B551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15180,10 +15180,10 @@
     <row r="549" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A549" s="6"/>
       <c r="B549" s="8" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C549" s="7" t="s">
         <v>2105</v>
-      </c>
-      <c r="C549" s="7" t="s">
-        <v>2106</v>
       </c>
       <c r="D549" s="6"/>
       <c r="E549" s="6"/>
@@ -15191,16 +15191,160 @@
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A550" s="6"/>
       <c r="B550" s="6" t="s">
-        <v>2107</v>
+        <v>2108</v>
       </c>
       <c r="C550" s="7" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
       <c r="D550" s="6"/>
       <c r="E550" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="160">
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="D112:D113"/>
+    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="B139:B140"/>
+    <mergeCell ref="C139:C140"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="D114:D115"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="E122:E123"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="C160:C161"/>
+    <mergeCell ref="D160:D161"/>
+    <mergeCell ref="E160:E161"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="C162:C163"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="D146:D147"/>
+    <mergeCell ref="E146:E147"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="C152:C153"/>
+    <mergeCell ref="D152:D153"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="D192:D193"/>
+    <mergeCell ref="E192:E193"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="C214:C215"/>
+    <mergeCell ref="D214:D215"/>
+    <mergeCell ref="E214:E215"/>
+    <mergeCell ref="B175:B176"/>
+    <mergeCell ref="C175:C176"/>
+    <mergeCell ref="D175:D176"/>
+    <mergeCell ref="E175:E176"/>
+    <mergeCell ref="B177:B178"/>
+    <mergeCell ref="C177:C178"/>
+    <mergeCell ref="D177:D178"/>
+    <mergeCell ref="E177:E178"/>
+    <mergeCell ref="B250:B251"/>
+    <mergeCell ref="C250:C251"/>
+    <mergeCell ref="D250:D251"/>
+    <mergeCell ref="E250:E251"/>
+    <mergeCell ref="B298:B299"/>
+    <mergeCell ref="C298:C299"/>
+    <mergeCell ref="D298:D299"/>
+    <mergeCell ref="E298:E299"/>
+    <mergeCell ref="B218:B219"/>
+    <mergeCell ref="C218:C219"/>
+    <mergeCell ref="D218:D219"/>
+    <mergeCell ref="E218:E219"/>
+    <mergeCell ref="B234:B235"/>
+    <mergeCell ref="C234:C235"/>
+    <mergeCell ref="D234:D235"/>
+    <mergeCell ref="E234:E235"/>
+    <mergeCell ref="B321:B322"/>
+    <mergeCell ref="C321:C322"/>
+    <mergeCell ref="D321:D322"/>
+    <mergeCell ref="E321:E322"/>
+    <mergeCell ref="B332:B333"/>
+    <mergeCell ref="C332:C333"/>
+    <mergeCell ref="D332:D333"/>
+    <mergeCell ref="E332:E333"/>
+    <mergeCell ref="B307:B308"/>
+    <mergeCell ref="C307:C308"/>
+    <mergeCell ref="D307:D308"/>
+    <mergeCell ref="E307:E308"/>
+    <mergeCell ref="B312:B313"/>
+    <mergeCell ref="C312:C313"/>
+    <mergeCell ref="D312:D313"/>
+    <mergeCell ref="E312:E313"/>
+    <mergeCell ref="B359:B360"/>
+    <mergeCell ref="C359:C360"/>
+    <mergeCell ref="D359:D360"/>
+    <mergeCell ref="E359:E360"/>
+    <mergeCell ref="B391:B392"/>
+    <mergeCell ref="C391:C392"/>
+    <mergeCell ref="D391:D392"/>
+    <mergeCell ref="E391:E392"/>
+    <mergeCell ref="B334:B335"/>
+    <mergeCell ref="C334:C335"/>
+    <mergeCell ref="D334:D335"/>
+    <mergeCell ref="E334:E335"/>
+    <mergeCell ref="B341:B342"/>
+    <mergeCell ref="C341:C342"/>
+    <mergeCell ref="D341:D342"/>
+    <mergeCell ref="E341:E342"/>
+    <mergeCell ref="B438:B439"/>
+    <mergeCell ref="C438:C439"/>
+    <mergeCell ref="D438:D439"/>
+    <mergeCell ref="E438:E439"/>
+    <mergeCell ref="B440:B441"/>
+    <mergeCell ref="C440:C441"/>
+    <mergeCell ref="D440:D441"/>
+    <mergeCell ref="E440:E441"/>
+    <mergeCell ref="B410:B411"/>
+    <mergeCell ref="C410:C411"/>
+    <mergeCell ref="D410:D411"/>
+    <mergeCell ref="E410:E411"/>
+    <mergeCell ref="B412:B413"/>
+    <mergeCell ref="C412:C413"/>
+    <mergeCell ref="D412:D413"/>
+    <mergeCell ref="E412:E413"/>
     <mergeCell ref="B525:B526"/>
     <mergeCell ref="C525:C526"/>
     <mergeCell ref="D525:D526"/>
@@ -15217,150 +15361,6 @@
     <mergeCell ref="C485:C486"/>
     <mergeCell ref="D485:D486"/>
     <mergeCell ref="E485:E486"/>
-    <mergeCell ref="B438:B439"/>
-    <mergeCell ref="C438:C439"/>
-    <mergeCell ref="D438:D439"/>
-    <mergeCell ref="E438:E439"/>
-    <mergeCell ref="B440:B441"/>
-    <mergeCell ref="C440:C441"/>
-    <mergeCell ref="D440:D441"/>
-    <mergeCell ref="E440:E441"/>
-    <mergeCell ref="B410:B411"/>
-    <mergeCell ref="C410:C411"/>
-    <mergeCell ref="D410:D411"/>
-    <mergeCell ref="E410:E411"/>
-    <mergeCell ref="B412:B413"/>
-    <mergeCell ref="C412:C413"/>
-    <mergeCell ref="D412:D413"/>
-    <mergeCell ref="E412:E413"/>
-    <mergeCell ref="B359:B360"/>
-    <mergeCell ref="C359:C360"/>
-    <mergeCell ref="D359:D360"/>
-    <mergeCell ref="E359:E360"/>
-    <mergeCell ref="B391:B392"/>
-    <mergeCell ref="C391:C392"/>
-    <mergeCell ref="D391:D392"/>
-    <mergeCell ref="E391:E392"/>
-    <mergeCell ref="B334:B335"/>
-    <mergeCell ref="C334:C335"/>
-    <mergeCell ref="D334:D335"/>
-    <mergeCell ref="E334:E335"/>
-    <mergeCell ref="B341:B342"/>
-    <mergeCell ref="C341:C342"/>
-    <mergeCell ref="D341:D342"/>
-    <mergeCell ref="E341:E342"/>
-    <mergeCell ref="B321:B322"/>
-    <mergeCell ref="C321:C322"/>
-    <mergeCell ref="D321:D322"/>
-    <mergeCell ref="E321:E322"/>
-    <mergeCell ref="B332:B333"/>
-    <mergeCell ref="C332:C333"/>
-    <mergeCell ref="D332:D333"/>
-    <mergeCell ref="E332:E333"/>
-    <mergeCell ref="B307:B308"/>
-    <mergeCell ref="C307:C308"/>
-    <mergeCell ref="D307:D308"/>
-    <mergeCell ref="E307:E308"/>
-    <mergeCell ref="B312:B313"/>
-    <mergeCell ref="C312:C313"/>
-    <mergeCell ref="D312:D313"/>
-    <mergeCell ref="E312:E313"/>
-    <mergeCell ref="B250:B251"/>
-    <mergeCell ref="C250:C251"/>
-    <mergeCell ref="D250:D251"/>
-    <mergeCell ref="E250:E251"/>
-    <mergeCell ref="B298:B299"/>
-    <mergeCell ref="C298:C299"/>
-    <mergeCell ref="D298:D299"/>
-    <mergeCell ref="E298:E299"/>
-    <mergeCell ref="B218:B219"/>
-    <mergeCell ref="C218:C219"/>
-    <mergeCell ref="D218:D219"/>
-    <mergeCell ref="E218:E219"/>
-    <mergeCell ref="B234:B235"/>
-    <mergeCell ref="C234:C235"/>
-    <mergeCell ref="D234:D235"/>
-    <mergeCell ref="E234:E235"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="C192:C193"/>
-    <mergeCell ref="D192:D193"/>
-    <mergeCell ref="E192:E193"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="C214:C215"/>
-    <mergeCell ref="D214:D215"/>
-    <mergeCell ref="E214:E215"/>
-    <mergeCell ref="B175:B176"/>
-    <mergeCell ref="C175:C176"/>
-    <mergeCell ref="D175:D176"/>
-    <mergeCell ref="E175:E176"/>
-    <mergeCell ref="B177:B178"/>
-    <mergeCell ref="C177:C178"/>
-    <mergeCell ref="D177:D178"/>
-    <mergeCell ref="E177:E178"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="C160:C161"/>
-    <mergeCell ref="D160:D161"/>
-    <mergeCell ref="E160:E161"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="C162:C163"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="B146:B147"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="D146:D147"/>
-    <mergeCell ref="E146:E147"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="C152:C153"/>
-    <mergeCell ref="D152:D153"/>
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="B139:B140"/>
-    <mergeCell ref="C139:C140"/>
-    <mergeCell ref="D139:D140"/>
-    <mergeCell ref="E139:E140"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="C114:C115"/>
-    <mergeCell ref="D114:D115"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="D122:D123"/>
-    <mergeCell ref="E122:E123"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="D112:D113"/>
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>